<commit_message>
added default selected data in regresyonDecider
</commit_message>
<xml_diff>
--- a/veriSeti2.xlsx
+++ b/veriSeti2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BATUHAN\Desktop\Korelasyon-Regresyon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB8E1E7-9F4C-4ACE-9A87-5EFD1DB9C136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15F7137-D71A-40C1-A616-9995524D8041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,9 +150,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,17 +430,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="13" max="13" width="8.88671875" customWidth="1"/>
@@ -459,13 +456,13 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -478,14 +475,14 @@
       <c r="B2" s="2">
         <v>30</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>125</v>
+      </c>
+      <c r="D2">
+        <v>148</v>
+      </c>
+      <c r="E2" s="1">
         <v>100</v>
-      </c>
-      <c r="D2">
-        <v>125</v>
-      </c>
-      <c r="E2">
-        <v>148</v>
       </c>
       <c r="F2" s="1">
         <v>5.5</v>
@@ -498,14 +495,14 @@
       <c r="B3" s="2">
         <v>35</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>132</v>
+      </c>
+      <c r="D3">
+        <v>148</v>
+      </c>
+      <c r="E3" s="1">
         <v>110</v>
-      </c>
-      <c r="D3">
-        <v>132</v>
-      </c>
-      <c r="E3">
-        <v>148</v>
       </c>
       <c r="F3" s="1">
         <v>5.8</v>
@@ -518,14 +515,14 @@
       <c r="B4" s="2">
         <v>22</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <v>134</v>
+      </c>
+      <c r="D4">
+        <v>148</v>
+      </c>
+      <c r="E4" s="1">
         <v>112</v>
-      </c>
-      <c r="D4">
-        <v>134</v>
-      </c>
-      <c r="E4">
-        <v>148</v>
       </c>
       <c r="F4" s="1">
         <v>6</v>
@@ -538,14 +535,14 @@
       <c r="B5" s="2">
         <v>29</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>148</v>
+      </c>
+      <c r="E5" s="1">
         <v>115</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <v>148</v>
       </c>
       <c r="F5" s="1">
         <v>5.9</v>
@@ -560,14 +557,14 @@
       <c r="B6" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <v>122</v>
+      </c>
+      <c r="D6">
+        <v>148</v>
+      </c>
+      <c r="E6" s="1">
         <v>117</v>
-      </c>
-      <c r="D6">
-        <v>122</v>
-      </c>
-      <c r="E6">
-        <v>148</v>
       </c>
       <c r="F6" s="1">
         <v>6.2</v>
@@ -580,14 +577,14 @@
       <c r="B7" s="2">
         <v>38</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
+        <v>145</v>
+      </c>
+      <c r="D7">
+        <v>148</v>
+      </c>
+      <c r="E7" s="1">
         <v>116</v>
-      </c>
-      <c r="D7">
-        <v>145</v>
-      </c>
-      <c r="E7">
-        <v>148</v>
       </c>
       <c r="F7" s="1">
         <v>6.3</v>
@@ -600,14 +597,14 @@
       <c r="B8" s="2">
         <v>40</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>148</v>
+      </c>
+      <c r="E8" s="1">
         <v>118</v>
-      </c>
-      <c r="D8">
-        <v>150</v>
-      </c>
-      <c r="E8">
-        <v>148</v>
       </c>
       <c r="F8" s="1">
         <v>6.5</v>
@@ -620,14 +617,14 @@
       <c r="B9" s="2">
         <v>43</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <v>148</v>
+      </c>
+      <c r="E9" s="1">
         <v>120</v>
-      </c>
-      <c r="D9">
-        <v>110</v>
-      </c>
-      <c r="E9">
-        <v>148</v>
       </c>
       <c r="F9" s="1">
         <v>6.6</v>
@@ -641,14 +638,14 @@
       <c r="B10" s="2">
         <v>32</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
+        <v>102</v>
+      </c>
+      <c r="D10">
+        <v>148</v>
+      </c>
+      <c r="E10" s="1">
         <v>121</v>
-      </c>
-      <c r="D10">
-        <v>102</v>
-      </c>
-      <c r="E10">
-        <v>148</v>
       </c>
       <c r="F10" s="1">
         <v>6.4</v>
@@ -663,14 +660,14 @@
       <c r="B11" s="2">
         <v>45</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
+        <v>111</v>
+      </c>
+      <c r="D11">
+        <v>148</v>
+      </c>
+      <c r="E11" s="1">
         <v>120</v>
-      </c>
-      <c r="D11">
-        <v>111</v>
-      </c>
-      <c r="E11">
-        <v>148</v>
       </c>
       <c r="F11" s="1">
         <v>6.5</v>
@@ -683,14 +680,14 @@
       <c r="B12" s="2">
         <v>50</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>148</v>
+      </c>
+      <c r="E12" s="1">
         <v>117</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12">
-        <v>148</v>
       </c>
       <c r="F12" s="1">
         <v>6.7</v>
@@ -703,69 +700,1571 @@
       <c r="B13" s="2">
         <v>20</v>
       </c>
-      <c r="C13" s="1">
-        <v>123</v>
+      <c r="C13">
+        <v>101</v>
       </c>
       <c r="D13">
-        <v>101</v>
-      </c>
-      <c r="E13">
-        <v>148</v>
+        <v>148</v>
+      </c>
+      <c r="E13" s="1">
+        <v>123</v>
       </c>
       <c r="F13" s="1">
         <v>6.8</v>
       </c>
     </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>101</v>
+      </c>
+      <c r="D14">
+        <v>148</v>
+      </c>
+      <c r="E14" s="1">
+        <v>123</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>101</v>
+      </c>
+      <c r="D15">
+        <v>148</v>
+      </c>
+      <c r="E15" s="1">
+        <v>123</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>101</v>
+      </c>
+      <c r="D16">
+        <v>148</v>
+      </c>
+      <c r="E16" s="1">
+        <v>123</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="9"/>
+      <c r="B17" s="2">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>101</v>
+      </c>
+      <c r="D17">
+        <v>148</v>
+      </c>
+      <c r="E17" s="1">
+        <v>123</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>101</v>
+      </c>
+      <c r="D18">
+        <v>148</v>
+      </c>
+      <c r="E18" s="1">
+        <v>123</v>
+      </c>
+      <c r="F18" s="1">
+        <v>6.8</v>
+      </c>
       <c r="N18" s="8"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="B19" s="2">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>101</v>
+      </c>
+      <c r="D19">
+        <v>148</v>
+      </c>
+      <c r="E19" s="1">
+        <v>123</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="B20" s="2">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>101</v>
+      </c>
+      <c r="D20">
+        <v>148</v>
+      </c>
+      <c r="E20" s="1">
+        <v>123</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>101</v>
+      </c>
+      <c r="D21">
+        <v>148</v>
+      </c>
+      <c r="E21" s="1">
+        <v>123</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6.8</v>
+      </c>
       <c r="J21" s="3"/>
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="B22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>101</v>
+      </c>
+      <c r="D22">
+        <v>148</v>
+      </c>
+      <c r="E22" s="1">
+        <v>123</v>
+      </c>
+      <c r="F22" s="1">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-      <c r="C23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>101</v>
+      </c>
+      <c r="D23">
+        <v>148</v>
+      </c>
+      <c r="E23" s="1">
+        <v>123</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-      <c r="C24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="B24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>101</v>
+      </c>
+      <c r="D24">
+        <v>148</v>
+      </c>
+      <c r="E24" s="1">
+        <v>123</v>
+      </c>
+      <c r="F24" s="1">
+        <v>6.8</v>
+      </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
-      <c r="C25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="B25" s="2">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>101</v>
+      </c>
+      <c r="D25">
+        <v>148</v>
+      </c>
+      <c r="E25" s="1">
+        <v>123</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6.8</v>
+      </c>
       <c r="J25" s="5"/>
       <c r="N25" s="6"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
-      <c r="C26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="B26" s="2">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>101</v>
+      </c>
+      <c r="D26">
+        <v>148</v>
+      </c>
+      <c r="E26" s="1">
+        <v>123</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>101</v>
+      </c>
+      <c r="D27">
+        <v>148</v>
+      </c>
+      <c r="E27" s="1">
+        <v>123</v>
+      </c>
+      <c r="F27" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>101</v>
+      </c>
+      <c r="D28">
+        <v>148</v>
+      </c>
+      <c r="E28" s="1">
+        <v>123</v>
+      </c>
+      <c r="F28" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>101</v>
+      </c>
+      <c r="D29">
+        <v>148</v>
+      </c>
+      <c r="E29" s="1">
+        <v>123</v>
+      </c>
+      <c r="F29" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>101</v>
+      </c>
+      <c r="D30">
+        <v>148</v>
+      </c>
+      <c r="E30" s="1">
+        <v>123</v>
+      </c>
+      <c r="F30" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>101</v>
+      </c>
+      <c r="D31">
+        <v>148</v>
+      </c>
+      <c r="E31" s="1">
+        <v>123</v>
+      </c>
+      <c r="F31" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>101</v>
+      </c>
+      <c r="D32">
+        <v>148</v>
+      </c>
+      <c r="E32" s="1">
+        <v>123</v>
+      </c>
+      <c r="F32" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>101</v>
+      </c>
+      <c r="D33">
+        <v>148</v>
+      </c>
+      <c r="E33" s="1">
+        <v>123</v>
+      </c>
+      <c r="F33" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>101</v>
+      </c>
+      <c r="D34">
+        <v>148</v>
+      </c>
+      <c r="E34" s="1">
+        <v>123</v>
+      </c>
+      <c r="F34" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>101</v>
+      </c>
+      <c r="D35">
+        <v>148</v>
+      </c>
+      <c r="E35" s="1">
+        <v>123</v>
+      </c>
+      <c r="F35" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>101</v>
+      </c>
+      <c r="D36">
+        <v>148</v>
+      </c>
+      <c r="E36" s="1">
+        <v>123</v>
+      </c>
+      <c r="F36" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>101</v>
+      </c>
+      <c r="D37">
+        <v>148</v>
+      </c>
+      <c r="E37" s="1">
+        <v>123</v>
+      </c>
+      <c r="F37" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>101</v>
+      </c>
+      <c r="D38">
+        <v>148</v>
+      </c>
+      <c r="E38" s="1">
+        <v>123</v>
+      </c>
+      <c r="F38" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>101</v>
+      </c>
+      <c r="D39">
+        <v>148</v>
+      </c>
+      <c r="E39" s="1">
+        <v>123</v>
+      </c>
+      <c r="F39" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>101</v>
+      </c>
+      <c r="D40">
+        <v>148</v>
+      </c>
+      <c r="E40" s="1">
+        <v>123</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>101</v>
+      </c>
+      <c r="D41">
+        <v>148</v>
+      </c>
+      <c r="E41" s="1">
+        <v>123</v>
+      </c>
+      <c r="F41" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>101</v>
+      </c>
+      <c r="D42">
+        <v>148</v>
+      </c>
+      <c r="E42" s="1">
+        <v>123</v>
+      </c>
+      <c r="F42" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
+        <v>20</v>
+      </c>
+      <c r="C43">
+        <v>101</v>
+      </c>
+      <c r="D43">
+        <v>148</v>
+      </c>
+      <c r="E43" s="1">
+        <v>123</v>
+      </c>
+      <c r="F43" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>20</v>
+      </c>
+      <c r="C44">
+        <v>101</v>
+      </c>
+      <c r="D44">
+        <v>148</v>
+      </c>
+      <c r="E44" s="1">
+        <v>123</v>
+      </c>
+      <c r="F44" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>101</v>
+      </c>
+      <c r="D45">
+        <v>148</v>
+      </c>
+      <c r="E45" s="1">
+        <v>123</v>
+      </c>
+      <c r="F45" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <v>101</v>
+      </c>
+      <c r="D46">
+        <v>148</v>
+      </c>
+      <c r="E46" s="1">
+        <v>123</v>
+      </c>
+      <c r="F46" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="2">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <v>101</v>
+      </c>
+      <c r="D47">
+        <v>148</v>
+      </c>
+      <c r="E47" s="1">
+        <v>123</v>
+      </c>
+      <c r="F47" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
+        <v>20</v>
+      </c>
+      <c r="C48">
+        <v>101</v>
+      </c>
+      <c r="D48">
+        <v>148</v>
+      </c>
+      <c r="E48" s="1">
+        <v>123</v>
+      </c>
+      <c r="F48" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="2">
+        <v>20</v>
+      </c>
+      <c r="C49">
+        <v>101</v>
+      </c>
+      <c r="D49">
+        <v>148</v>
+      </c>
+      <c r="E49" s="1">
+        <v>123</v>
+      </c>
+      <c r="F49" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>20</v>
+      </c>
+      <c r="C50">
+        <v>101</v>
+      </c>
+      <c r="D50">
+        <v>148</v>
+      </c>
+      <c r="E50" s="1">
+        <v>123</v>
+      </c>
+      <c r="F50" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>20</v>
+      </c>
+      <c r="C51">
+        <v>101</v>
+      </c>
+      <c r="D51">
+        <v>148</v>
+      </c>
+      <c r="E51" s="1">
+        <v>123</v>
+      </c>
+      <c r="F51" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="2">
+        <v>20</v>
+      </c>
+      <c r="C52">
+        <v>101</v>
+      </c>
+      <c r="D52">
+        <v>148</v>
+      </c>
+      <c r="E52" s="1">
+        <v>123</v>
+      </c>
+      <c r="F52" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="2">
+        <v>20</v>
+      </c>
+      <c r="C53">
+        <v>101</v>
+      </c>
+      <c r="D53">
+        <v>148</v>
+      </c>
+      <c r="E53" s="1">
+        <v>123</v>
+      </c>
+      <c r="F53" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="2">
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <v>101</v>
+      </c>
+      <c r="D54">
+        <v>148</v>
+      </c>
+      <c r="E54" s="1">
+        <v>123</v>
+      </c>
+      <c r="F54" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>20</v>
+      </c>
+      <c r="C55">
+        <v>101</v>
+      </c>
+      <c r="D55">
+        <v>148</v>
+      </c>
+      <c r="E55" s="1">
+        <v>123</v>
+      </c>
+      <c r="F55" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <v>101</v>
+      </c>
+      <c r="D56">
+        <v>148</v>
+      </c>
+      <c r="E56" s="1">
+        <v>123</v>
+      </c>
+      <c r="F56" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>20</v>
+      </c>
+      <c r="C57">
+        <v>101</v>
+      </c>
+      <c r="D57">
+        <v>148</v>
+      </c>
+      <c r="E57" s="1">
+        <v>123</v>
+      </c>
+      <c r="F57" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <v>101</v>
+      </c>
+      <c r="D58">
+        <v>148</v>
+      </c>
+      <c r="E58" s="1">
+        <v>123</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>101</v>
+      </c>
+      <c r="D59">
+        <v>148</v>
+      </c>
+      <c r="E59" s="1">
+        <v>123</v>
+      </c>
+      <c r="F59" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>101</v>
+      </c>
+      <c r="D60">
+        <v>148</v>
+      </c>
+      <c r="E60" s="1">
+        <v>123</v>
+      </c>
+      <c r="F60" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>101</v>
+      </c>
+      <c r="D61">
+        <v>148</v>
+      </c>
+      <c r="E61" s="1">
+        <v>123</v>
+      </c>
+      <c r="F61" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>20</v>
+      </c>
+      <c r="C62">
+        <v>101</v>
+      </c>
+      <c r="D62">
+        <v>148</v>
+      </c>
+      <c r="E62" s="1">
+        <v>123</v>
+      </c>
+      <c r="F62" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>101</v>
+      </c>
+      <c r="D63">
+        <v>148</v>
+      </c>
+      <c r="E63" s="1">
+        <v>123</v>
+      </c>
+      <c r="F63" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>20</v>
+      </c>
+      <c r="C64">
+        <v>101</v>
+      </c>
+      <c r="D64">
+        <v>148</v>
+      </c>
+      <c r="E64" s="1">
+        <v>123</v>
+      </c>
+      <c r="F64" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="2">
+        <v>20</v>
+      </c>
+      <c r="C65">
+        <v>101</v>
+      </c>
+      <c r="D65">
+        <v>148</v>
+      </c>
+      <c r="E65" s="1">
+        <v>123</v>
+      </c>
+      <c r="F65" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>20</v>
+      </c>
+      <c r="C66">
+        <v>101</v>
+      </c>
+      <c r="D66">
+        <v>148</v>
+      </c>
+      <c r="E66" s="1">
+        <v>123</v>
+      </c>
+      <c r="F66" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="2">
+        <v>20</v>
+      </c>
+      <c r="C67">
+        <v>101</v>
+      </c>
+      <c r="D67">
+        <v>148</v>
+      </c>
+      <c r="E67" s="1">
+        <v>123</v>
+      </c>
+      <c r="F67" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="2">
+        <v>20</v>
+      </c>
+      <c r="C68">
+        <v>101</v>
+      </c>
+      <c r="D68">
+        <v>148</v>
+      </c>
+      <c r="E68" s="1">
+        <v>123</v>
+      </c>
+      <c r="F68" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="2">
+        <v>20</v>
+      </c>
+      <c r="C69">
+        <v>101</v>
+      </c>
+      <c r="D69">
+        <v>148</v>
+      </c>
+      <c r="E69" s="1">
+        <v>123</v>
+      </c>
+      <c r="F69" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="2">
+        <v>20</v>
+      </c>
+      <c r="C70">
+        <v>101</v>
+      </c>
+      <c r="D70">
+        <v>148</v>
+      </c>
+      <c r="E70" s="1">
+        <v>123</v>
+      </c>
+      <c r="F70" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="2">
+        <v>20</v>
+      </c>
+      <c r="C71">
+        <v>101</v>
+      </c>
+      <c r="D71">
+        <v>148</v>
+      </c>
+      <c r="E71" s="1">
+        <v>123</v>
+      </c>
+      <c r="F71" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="2">
+        <v>20</v>
+      </c>
+      <c r="C72">
+        <v>101</v>
+      </c>
+      <c r="D72">
+        <v>148</v>
+      </c>
+      <c r="E72" s="1">
+        <v>123</v>
+      </c>
+      <c r="F72" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="2">
+        <v>20</v>
+      </c>
+      <c r="C73">
+        <v>101</v>
+      </c>
+      <c r="D73">
+        <v>148</v>
+      </c>
+      <c r="E73" s="1">
+        <v>123</v>
+      </c>
+      <c r="F73" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="2">
+        <v>20</v>
+      </c>
+      <c r="C74">
+        <v>101</v>
+      </c>
+      <c r="D74">
+        <v>148</v>
+      </c>
+      <c r="E74" s="1">
+        <v>123</v>
+      </c>
+      <c r="F74" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="2">
+        <v>20</v>
+      </c>
+      <c r="C75">
+        <v>101</v>
+      </c>
+      <c r="D75">
+        <v>148</v>
+      </c>
+      <c r="E75" s="1">
+        <v>123</v>
+      </c>
+      <c r="F75" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="2">
+        <v>20</v>
+      </c>
+      <c r="C76">
+        <v>101</v>
+      </c>
+      <c r="D76">
+        <v>148</v>
+      </c>
+      <c r="E76" s="1">
+        <v>123</v>
+      </c>
+      <c r="F76" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="2">
+        <v>20</v>
+      </c>
+      <c r="C77">
+        <v>101</v>
+      </c>
+      <c r="D77">
+        <v>148</v>
+      </c>
+      <c r="E77" s="1">
+        <v>123</v>
+      </c>
+      <c r="F77" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" s="2">
+        <v>20</v>
+      </c>
+      <c r="C78">
+        <v>101</v>
+      </c>
+      <c r="D78">
+        <v>148</v>
+      </c>
+      <c r="E78" s="1">
+        <v>123</v>
+      </c>
+      <c r="F78" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="2">
+        <v>20</v>
+      </c>
+      <c r="C79">
+        <v>101</v>
+      </c>
+      <c r="D79">
+        <v>148</v>
+      </c>
+      <c r="E79" s="1">
+        <v>123</v>
+      </c>
+      <c r="F79" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" s="2">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>101</v>
+      </c>
+      <c r="D80">
+        <v>148</v>
+      </c>
+      <c r="E80" s="1">
+        <v>123</v>
+      </c>
+      <c r="F80" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81" s="2">
+        <v>20</v>
+      </c>
+      <c r="C81">
+        <v>101</v>
+      </c>
+      <c r="D81">
+        <v>148</v>
+      </c>
+      <c r="E81" s="1">
+        <v>123</v>
+      </c>
+      <c r="F81" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B82" s="2">
+        <v>20</v>
+      </c>
+      <c r="C82">
+        <v>101</v>
+      </c>
+      <c r="D82">
+        <v>148</v>
+      </c>
+      <c r="E82" s="1">
+        <v>123</v>
+      </c>
+      <c r="F82" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B83" s="2">
+        <v>20</v>
+      </c>
+      <c r="C83">
+        <v>101</v>
+      </c>
+      <c r="D83">
+        <v>148</v>
+      </c>
+      <c r="E83" s="1">
+        <v>123</v>
+      </c>
+      <c r="F83" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B84" s="2">
+        <v>20</v>
+      </c>
+      <c r="C84">
+        <v>101</v>
+      </c>
+      <c r="D84">
+        <v>148</v>
+      </c>
+      <c r="E84" s="1">
+        <v>123</v>
+      </c>
+      <c r="F84" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B85" s="2">
+        <v>20</v>
+      </c>
+      <c r="C85">
+        <v>101</v>
+      </c>
+      <c r="D85">
+        <v>148</v>
+      </c>
+      <c r="E85" s="1">
+        <v>123</v>
+      </c>
+      <c r="F85" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B86" s="2">
+        <v>20</v>
+      </c>
+      <c r="C86">
+        <v>101</v>
+      </c>
+      <c r="D86">
+        <v>148</v>
+      </c>
+      <c r="E86" s="1">
+        <v>123</v>
+      </c>
+      <c r="F86" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="2">
+        <v>20</v>
+      </c>
+      <c r="C87">
+        <v>101</v>
+      </c>
+      <c r="D87">
+        <v>148</v>
+      </c>
+      <c r="E87" s="1">
+        <v>123</v>
+      </c>
+      <c r="F87" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88" s="2">
+        <v>20</v>
+      </c>
+      <c r="C88">
+        <v>101</v>
+      </c>
+      <c r="D88">
+        <v>148</v>
+      </c>
+      <c r="E88" s="1">
+        <v>123</v>
+      </c>
+      <c r="F88" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B89" s="2">
+        <v>20</v>
+      </c>
+      <c r="C89">
+        <v>101</v>
+      </c>
+      <c r="D89">
+        <v>148</v>
+      </c>
+      <c r="E89" s="1">
+        <v>123</v>
+      </c>
+      <c r="F89" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" s="2">
+        <v>20</v>
+      </c>
+      <c r="C90">
+        <v>101</v>
+      </c>
+      <c r="D90">
+        <v>148</v>
+      </c>
+      <c r="E90" s="1">
+        <v>123</v>
+      </c>
+      <c r="F90" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B91" s="2">
+        <v>20</v>
+      </c>
+      <c r="C91">
+        <v>101</v>
+      </c>
+      <c r="D91">
+        <v>148</v>
+      </c>
+      <c r="E91" s="1">
+        <v>123</v>
+      </c>
+      <c r="F91" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B92" s="2">
+        <v>20</v>
+      </c>
+      <c r="C92">
+        <v>101</v>
+      </c>
+      <c r="D92">
+        <v>148</v>
+      </c>
+      <c r="E92" s="1">
+        <v>123</v>
+      </c>
+      <c r="F92" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B93" s="2">
+        <v>20</v>
+      </c>
+      <c r="C93">
+        <v>101</v>
+      </c>
+      <c r="D93">
+        <v>148</v>
+      </c>
+      <c r="E93" s="1">
+        <v>123</v>
+      </c>
+      <c r="F93" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B94" s="2">
+        <v>20</v>
+      </c>
+      <c r="C94">
+        <v>101</v>
+      </c>
+      <c r="D94">
+        <v>148</v>
+      </c>
+      <c r="E94" s="1">
+        <v>123</v>
+      </c>
+      <c r="F94" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B95" s="2">
+        <v>20</v>
+      </c>
+      <c r="C95">
+        <v>101</v>
+      </c>
+      <c r="D95">
+        <v>148</v>
+      </c>
+      <c r="E95" s="1">
+        <v>123</v>
+      </c>
+      <c r="F95" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B96" s="2">
+        <v>20</v>
+      </c>
+      <c r="C96">
+        <v>101</v>
+      </c>
+      <c r="D96">
+        <v>148</v>
+      </c>
+      <c r="E96" s="1">
+        <v>123</v>
+      </c>
+      <c r="F96" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B97" s="2">
+        <v>20</v>
+      </c>
+      <c r="C97">
+        <v>101</v>
+      </c>
+      <c r="D97">
+        <v>148</v>
+      </c>
+      <c r="E97" s="1">
+        <v>123</v>
+      </c>
+      <c r="F97" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B98" s="2">
+        <v>20</v>
+      </c>
+      <c r="C98">
+        <v>101</v>
+      </c>
+      <c r="D98">
+        <v>148</v>
+      </c>
+      <c r="E98" s="1">
+        <v>123</v>
+      </c>
+      <c r="F98" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B99" s="2">
+        <v>20</v>
+      </c>
+      <c r="C99">
+        <v>101</v>
+      </c>
+      <c r="D99">
+        <v>148</v>
+      </c>
+      <c r="E99" s="1">
+        <v>123</v>
+      </c>
+      <c r="F99" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B100" s="2">
+        <v>20</v>
+      </c>
+      <c r="C100">
+        <v>101</v>
+      </c>
+      <c r="D100">
+        <v>148</v>
+      </c>
+      <c r="E100" s="1">
+        <v>123</v>
+      </c>
+      <c r="F100" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B101" s="2">
+        <v>20</v>
+      </c>
+      <c r="C101">
+        <v>101</v>
+      </c>
+      <c r="D101">
+        <v>148</v>
+      </c>
+      <c r="E101" s="1">
+        <v>123</v>
+      </c>
+      <c r="F101" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B102" s="2">
+        <v>20</v>
+      </c>
+      <c r="C102">
+        <v>101</v>
+      </c>
+      <c r="D102">
+        <v>148</v>
+      </c>
+      <c r="E102" s="1">
+        <v>123</v>
+      </c>
+      <c r="F102" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B103" s="2">
+        <v>20</v>
+      </c>
+      <c r="C103">
+        <v>101</v>
+      </c>
+      <c r="D103">
+        <v>148</v>
+      </c>
+      <c r="E103" s="1">
+        <v>123</v>
+      </c>
+      <c r="F103" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B104" s="2">
+        <v>20</v>
+      </c>
+      <c r="C104">
+        <v>101</v>
+      </c>
+      <c r="D104">
+        <v>148</v>
+      </c>
+      <c r="E104" s="1">
+        <v>123</v>
+      </c>
+      <c r="F104" s="1">
+        <v>6.8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>